<commit_message>
S04P12A401-111 [+] Edit DB recipe 통
</commit_message>
<xml_diff>
--- a/DB/cocktailDB/cocktailDB_byNamu_Tequila, Rum, Brandy, NonAlcohol.xlsx
+++ b/DB/cocktailDB/cocktailDB_byNamu_Tequila, Rum, Brandy, NonAlcohol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\multicampus\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\multicampus\Desktop\s04p12a401\DB\cocktailDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="430">
   <si>
     <t>기저주류</t>
   </si>
@@ -214,9 +214,6 @@
   </si>
   <si>
     <t>토닉워터</t>
-  </si>
-  <si>
-    <t>재료를 모두 하이볼 글래스에 빌드한 다음, 레몬으로 가니쉬하면 완성.</t>
   </si>
   <si>
     <t>롱 아일랜드 아이스 티</t>
@@ -236,9 +233,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>드라이 진</t>
-  </si>
-  <si>
     <t>보드카</t>
   </si>
   <si>
@@ -248,13 +242,7 @@
     <t xml:space="preserve">데킬라 </t>
   </si>
   <si>
-    <t>검 시럽</t>
-  </si>
-  <si>
     <t>콜라</t>
-  </si>
-  <si>
-    <t>레몬 트위스트</t>
   </si>
   <si>
     <t>마가리타</t>
@@ -1478,9 +1466,6 @@
     <t xml:space="preserve"> 1tsp</t>
   </si>
   <si>
-    <t>아즈텍 블러드</t>
-  </si>
-  <si>
     <t>데킬라 베이스로, B-52같은 레이어드 슈터 칵테일이다.
 아즈텍의 피라는 이름에 걸맞게 강렬한 칵테일이다. 이름 때문인지 색도 이름처럼 핏빛이다.</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -1492,9 +1477,6 @@
     <t>1/3oz (10ml)</t>
   </si>
   <si>
-    <t>하바네로 소스</t>
-  </si>
-  <si>
     <t>엘 디아블로</t>
   </si>
   <si>
@@ -1514,9 +1496,6 @@
   </si>
   <si>
     <t>2~3oz (60~90ml)</t>
-  </si>
-  <si>
-    <t>엘 토로 로코</t>
   </si>
   <si>
     <t>데킬라 베이스로, 동명의 몬스터 트럭에서 이름을 따온 칵테일이고 스폰서인 레드불의 홍보용으로 만들어진 칵테일이다.</t>
@@ -2712,6 +2691,54 @@
   </si>
   <si>
     <t>2 dash</t>
+  </si>
+  <si>
+    <t>재료를 모두 하이볼 글래스에 빌드한 다음, 레몬으로 가니쉬하면 완성.</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 1/2oz (45ml)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>full up</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>진</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>아즈텍 마티니</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 oz (60ml)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>깔루아</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>자몽 주스</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 oz</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">꿀 </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>약간</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>엘 토로 로코</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3145,16 +3172,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D76" workbookViewId="0">
-      <selection activeCell="M76" sqref="M76"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="19.69921875" customWidth="1"/>
     <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="87.796875" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="11.59765625" customWidth="1"/>
+    <col min="4" max="4" width="18.59765625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="14.59765625" customWidth="1"/>
     <col min="7" max="7" width="15.19921875" customWidth="1"/>
@@ -3173,7 +3200,7 @@
     <col min="21" max="21" width="13.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3193,7 +3220,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="104.4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -3219,7 +3246,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="87" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -3248,7 +3275,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="365.4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -3277,7 +3304,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="121.8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>27</v>
       </c>
@@ -3306,7 +3333,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="52.2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>33</v>
       </c>
@@ -3341,7 +3368,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="208.8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>41</v>
       </c>
@@ -3364,7 +3391,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="52.2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>47</v>
       </c>
@@ -3372,7 +3399,7 @@
         <v>48</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>53</v>
+        <v>418</v>
       </c>
       <c r="E8" t="s">
         <v>49</v>
@@ -3387,36 +3414,36 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="400.2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>421</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H9" t="s">
         <v>8</v>
       </c>
       <c r="I9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J9" t="s">
         <v>8</v>
       </c>
       <c r="K9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L9" t="s">
         <v>8</v>
@@ -3431,36 +3458,27 @@
         <v>16</v>
       </c>
       <c r="P9" t="s">
-        <v>30</v>
+        <v>419</v>
       </c>
       <c r="Q9" t="s">
+        <v>59</v>
+      </c>
+      <c r="R9" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="R9" t="s">
-        <v>38</v>
-      </c>
-      <c r="S9" t="s">
+      <c r="D10" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="T9" t="s">
-        <v>40</v>
-      </c>
-      <c r="U9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="348" x14ac:dyDescent="0.4">
-      <c r="B10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
         <v>38</v>
@@ -3472,30 +3490,30 @@
         <v>8</v>
       </c>
       <c r="I10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="139.19999999999999" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F11" t="s">
         <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H11" t="s">
         <v>22</v>
@@ -3507,15 +3525,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="69.599999999999994" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
@@ -3524,27 +3542,27 @@
         <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="52.2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
@@ -3553,30 +3571,30 @@
         <v>38</v>
       </c>
       <c r="G13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H13" t="s">
         <v>8</v>
       </c>
       <c r="I13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F14" t="s">
         <v>38</v>
@@ -3594,7 +3612,7 @@
         <v>8</v>
       </c>
       <c r="K14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L14" t="s">
         <v>18</v>
@@ -3606,15 +3624,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="121.8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
@@ -3623,33 +3641,33 @@
         <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H15" t="s">
         <v>38</v>
       </c>
       <c r="I15" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="52.2" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G16" t="s">
         <v>37</v>
@@ -3658,21 +3676,21 @@
         <v>38</v>
       </c>
       <c r="I16" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="J16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="52.2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
@@ -3681,7 +3699,7 @@
         <v>22</v>
       </c>
       <c r="G17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H17" t="s">
         <v>24</v>
@@ -3693,33 +3711,33 @@
         <v>18</v>
       </c>
       <c r="K17" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="L17" t="s">
         <v>18</v>
       </c>
       <c r="M17" t="s">
+        <v>95</v>
+      </c>
+      <c r="N17" t="s">
+        <v>96</v>
+      </c>
+      <c r="O17" t="s">
+        <v>97</v>
+      </c>
+      <c r="P17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="N17" t="s">
+      <c r="D18" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="O17" t="s">
-        <v>101</v>
-      </c>
-      <c r="P17" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="87" x14ac:dyDescent="0.4">
-      <c r="B18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
@@ -3728,7 +3746,7 @@
         <v>38</v>
       </c>
       <c r="G18" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H18" t="s">
         <v>8</v>
@@ -3740,18 +3758,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="87" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
         <v>50</v>
@@ -3760,33 +3778,33 @@
         <v>25</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="69.599999999999994" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F20" t="s">
         <v>36</v>
       </c>
       <c r="G20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H20" t="s">
         <v>38</v>
@@ -3801,82 +3819,88 @@
         <v>25</v>
       </c>
       <c r="L20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" t="s">
+        <v>422</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" t="s">
+        <v>423</v>
+      </c>
+      <c r="G21" t="s">
+        <v>424</v>
+      </c>
+      <c r="H21" t="s">
+        <v>423</v>
+      </c>
+      <c r="I21" t="s">
+        <v>425</v>
+      </c>
+      <c r="J21" t="s">
+        <v>426</v>
+      </c>
+      <c r="K21" t="s">
+        <v>427</v>
+      </c>
+      <c r="L21" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" ht="52.2" x14ac:dyDescent="0.4">
-      <c r="B21" t="s">
+      <c r="C22" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E21" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" t="s">
-        <v>118</v>
-      </c>
-      <c r="G21" t="s">
-        <v>97</v>
-      </c>
-      <c r="H21" t="s">
-        <v>118</v>
-      </c>
-      <c r="I21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J21" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="104.4" x14ac:dyDescent="0.4">
-      <c r="B22" t="s">
-        <v>120</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F22" t="s">
         <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H22" t="s">
         <v>8</v>
       </c>
       <c r="I22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J22" t="s">
         <v>8</v>
       </c>
       <c r="K22" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="L22" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="69.599999999999994" x14ac:dyDescent="0.4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
-        <v>126</v>
+        <v>429</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E23" t="s">
         <v>7</v>
@@ -3885,59 +3909,59 @@
         <v>38</v>
       </c>
       <c r="G23" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="H23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="104.4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F24" t="s">
         <v>22</v>
       </c>
       <c r="G24" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H24" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="I24" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="J24" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" ht="104.4" x14ac:dyDescent="0.4">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F25" t="s">
         <v>22</v>
       </c>
       <c r="G25" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="H25" t="s">
         <v>38</v>
@@ -3946,27 +3970,27 @@
         <v>16</v>
       </c>
       <c r="J25" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="K25" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="L25" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" ht="191.4" x14ac:dyDescent="0.4">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F26" t="s">
         <v>22</v>
@@ -3978,179 +4002,179 @@
         <v>8</v>
       </c>
       <c r="I26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J26" t="s">
         <v>8</v>
       </c>
       <c r="K26" t="s">
+        <v>136</v>
+      </c>
+      <c r="L26" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B27" t="s">
+        <v>144</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" t="s">
+        <v>141</v>
+      </c>
+      <c r="G27" t="s">
+        <v>142</v>
+      </c>
+      <c r="H27" t="s">
         <v>143</v>
       </c>
-      <c r="L26" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="174" x14ac:dyDescent="0.4">
-      <c r="B27" t="s">
-        <v>151</v>
-      </c>
-      <c r="C27" s="3" t="s">
+    </row>
+    <row r="28" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E27" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" t="s">
-        <v>148</v>
-      </c>
-      <c r="G27" t="s">
-        <v>149</v>
-      </c>
-      <c r="H27" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" ht="69.599999999999994" x14ac:dyDescent="0.4">
-      <c r="B28" t="s">
-        <v>152</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="E28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F28" t="s">
         <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="H28" t="s">
         <v>15</v>
       </c>
       <c r="I28" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="J28" t="s">
         <v>15</v>
       </c>
       <c r="K28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L28" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="M28" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="N28" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="O28" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="P28" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="Q28" t="s">
         <v>39</v>
       </c>
       <c r="R28" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="S28" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="T28" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" ht="156.6" x14ac:dyDescent="0.4">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F29" t="s">
         <v>15</v>
       </c>
       <c r="G29" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H29" t="s">
         <v>8</v>
       </c>
       <c r="I29" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J29" t="s">
         <v>38</v>
       </c>
       <c r="K29" t="s">
+        <v>159</v>
+      </c>
+      <c r="L29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" t="s">
+        <v>161</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E30" t="s">
+        <v>165</v>
+      </c>
+      <c r="F30" t="s">
         <v>166</v>
       </c>
-      <c r="L29" t="s">
+      <c r="G30" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" ht="139.19999999999999" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
+      <c r="H30" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B31" t="s">
         <v>169</v>
       </c>
-      <c r="B30" t="s">
-        <v>168</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="E30" t="s">
-        <v>172</v>
-      </c>
-      <c r="F30" t="s">
-        <v>173</v>
-      </c>
-      <c r="G30" t="s">
-        <v>174</v>
-      </c>
-      <c r="H30" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" ht="191.4" x14ac:dyDescent="0.4">
-      <c r="B31" t="s">
-        <v>176</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="E31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F31" t="s">
         <v>38</v>
       </c>
       <c r="G31" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="H31" t="s">
         <v>8</v>
@@ -4162,105 +4186,105 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="409.6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E32" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F32" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="G32" t="s">
         <v>17</v>
       </c>
       <c r="H32" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="I32" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="33" spans="2:24" ht="121.8" x14ac:dyDescent="0.4">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E33" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="F33" t="s">
         <v>15</v>
       </c>
       <c r="G33" t="s">
+        <v>183</v>
+      </c>
+      <c r="H33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I33" t="s">
+        <v>184</v>
+      </c>
+      <c r="J33" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B34" t="s">
+        <v>187</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E34" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" t="s">
         <v>190</v>
       </c>
-      <c r="H33" t="s">
-        <v>135</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="G34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H34" t="s">
         <v>191</v>
       </c>
-      <c r="J33" t="s">
+      <c r="I34" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="34" spans="2:24" ht="313.2" x14ac:dyDescent="0.4">
-      <c r="B34" t="s">
+      <c r="J34" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="35" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B35" t="s">
         <v>194</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="E35" t="s">
         <v>196</v>
-      </c>
-      <c r="E34" t="s">
-        <v>59</v>
-      </c>
-      <c r="F34" t="s">
-        <v>197</v>
-      </c>
-      <c r="G34" t="s">
-        <v>67</v>
-      </c>
-      <c r="H34" t="s">
-        <v>198</v>
-      </c>
-      <c r="I34" t="s">
-        <v>199</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="35" spans="2:24" ht="174" x14ac:dyDescent="0.4">
-      <c r="B35" t="s">
-        <v>201</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="E35" t="s">
-        <v>203</v>
       </c>
       <c r="F35" t="s">
         <v>22</v>
       </c>
       <c r="G35" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H35" t="s">
         <v>22</v>
@@ -4272,164 +4296,164 @@
         <v>18</v>
       </c>
       <c r="K35" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="L35" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="2:24" ht="156.6" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F36" t="s">
         <v>22</v>
       </c>
       <c r="G36" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H36" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="I36" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="J36" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:24" ht="52.2" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B37" s="3" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C37" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="E37" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="F37" t="s">
         <v>15</v>
       </c>
       <c r="G37" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="H37" t="s">
         <v>8</v>
       </c>
       <c r="I37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J37" t="s">
         <v>29</v>
       </c>
       <c r="K37" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="L37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="2:24" ht="121.8" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B38" s="3" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C38" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E38" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F38" t="s">
         <v>15</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H38" t="s">
         <v>31</v>
       </c>
       <c r="I38" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="J38" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="K38" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="L38" t="s">
         <v>8</v>
       </c>
       <c r="M38" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="N38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="2:24" ht="208.8" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
+        <v>210</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E39" t="s">
+        <v>213</v>
+      </c>
+      <c r="F39" t="s">
+        <v>154</v>
+      </c>
+      <c r="G39" t="s">
+        <v>214</v>
+      </c>
+      <c r="H39" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="40" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B40" t="s">
+        <v>216</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="D39" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E39" t="s">
-        <v>220</v>
-      </c>
-      <c r="F39" t="s">
-        <v>161</v>
-      </c>
-      <c r="G39" t="s">
-        <v>221</v>
-      </c>
-      <c r="H39" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="40" spans="2:24" ht="121.8" x14ac:dyDescent="0.4">
-      <c r="B40" t="s">
-        <v>223</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>226</v>
-      </c>
       <c r="E40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F40" t="s">
         <v>29</v>
       </c>
       <c r="G40" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="H40" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="I40" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J40" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="K40" t="s">
         <v>37</v>
@@ -4438,33 +4462,33 @@
         <v>8</v>
       </c>
       <c r="M40" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="N40" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="2:24" ht="87" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C41" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="E41" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F41" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G41" t="s">
         <v>37</v>
       </c>
       <c r="H41" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="I41" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J41" t="s">
         <v>38</v>
@@ -4476,80 +4500,80 @@
         <v>38</v>
       </c>
       <c r="M41" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="N41" t="s">
         <v>38</v>
       </c>
       <c r="O41" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="P41" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="42" spans="2:24" ht="409.6" x14ac:dyDescent="0.4">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="E42" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="F42" t="s">
         <v>22</v>
       </c>
       <c r="G42" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="H42" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="I42" t="s">
         <v>17</v>
       </c>
       <c r="J42" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="K42" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="L42" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="M42" t="s">
         <v>44</v>
       </c>
       <c r="N42" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="43" spans="2:24" ht="87" x14ac:dyDescent="0.4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F43" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G43" t="s">
         <v>16</v>
       </c>
       <c r="H43" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="I43" t="s">
         <v>25</v>
@@ -4558,30 +4582,30 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="2:24" ht="121.8" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E44" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F44" t="s">
         <v>38</v>
       </c>
       <c r="G44" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="H44" t="s">
         <v>38</v>
       </c>
       <c r="I44" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="J44" t="s">
         <v>38</v>
@@ -4593,124 +4617,124 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="2:24" ht="87" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="E45" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F45" t="s">
         <v>38</v>
       </c>
       <c r="G45" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H45" t="s">
         <v>8</v>
       </c>
       <c r="I45" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="J45" t="s">
         <v>38</v>
       </c>
       <c r="K45" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="L45" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="2:24" ht="69.599999999999994" x14ac:dyDescent="0.4">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="E46" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F46" t="s">
         <v>38</v>
       </c>
       <c r="G46" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H46" t="s">
         <v>38</v>
       </c>
       <c r="I46" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="J46" t="s">
         <v>36</v>
       </c>
       <c r="K46" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="L46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="2:24" ht="226.2" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B47" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C47" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>262</v>
-      </c>
       <c r="E47" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="F47" t="s">
         <v>22</v>
       </c>
       <c r="G47" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="H47" t="s">
         <v>22</v>
       </c>
       <c r="I47" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="J47" t="s">
         <v>38</v>
       </c>
       <c r="K47" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="L47" t="s">
         <v>8</v>
       </c>
       <c r="M47" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="N47" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="O47" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P47" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="Q47" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="R47" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="S47" t="s">
         <v>25</v>
@@ -4719,185 +4743,185 @@
         <v>18</v>
       </c>
       <c r="U47" s="3" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="V47" t="s">
         <v>40</v>
       </c>
       <c r="W47" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="X47" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="2:24" ht="174" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B48" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="E48" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="F48" t="s">
         <v>22</v>
       </c>
       <c r="G48" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="H48" t="s">
         <v>8</v>
       </c>
       <c r="I48" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J48" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:22" ht="156.6" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B49" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="E49" t="s">
+        <v>57</v>
+      </c>
+      <c r="F49" t="s">
+        <v>235</v>
+      </c>
+      <c r="G49" t="s">
+        <v>63</v>
+      </c>
+      <c r="H49" t="s">
+        <v>113</v>
+      </c>
+      <c r="I49" t="s">
         <v>59</v>
       </c>
-      <c r="F49" t="s">
-        <v>242</v>
-      </c>
-      <c r="G49" t="s">
-        <v>67</v>
-      </c>
-      <c r="H49" t="s">
-        <v>118</v>
-      </c>
-      <c r="I49" t="s">
-        <v>62</v>
-      </c>
       <c r="J49" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="50" spans="1:22" ht="243.6" x14ac:dyDescent="0.4">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B50" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E50" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F50" t="s">
         <v>38</v>
       </c>
       <c r="G50" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H50" t="s">
         <v>38</v>
       </c>
       <c r="I50" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="J50" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="K50" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="L50" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="51" spans="1:22" ht="365.4" x14ac:dyDescent="0.4">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B51" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="E51" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F51" t="s">
         <v>15</v>
       </c>
       <c r="G51" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="H51" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="I51" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="J51" t="s">
         <v>18</v>
       </c>
       <c r="K51" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="L51" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="M51" t="s">
         <v>17</v>
       </c>
       <c r="N51" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="O51" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="P51" t="s">
         <v>18</v>
       </c>
       <c r="Q51" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="R51" t="s">
         <v>18</v>
       </c>
       <c r="S51" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="T51" t="s">
         <v>18</v>
       </c>
       <c r="U51" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="V51" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:22" ht="87" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B52" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="E52" t="s">
         <v>25</v>
@@ -4906,77 +4930,77 @@
         <v>38</v>
       </c>
       <c r="G52" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H52" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="I52" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="J52" t="s">
         <v>15</v>
       </c>
       <c r="K52" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="L52" t="s">
         <v>38</v>
       </c>
       <c r="M52" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="N52" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:22" ht="121.8" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B53" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E53" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="F53" t="s">
         <v>38</v>
       </c>
       <c r="G53" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H53" t="s">
         <v>8</v>
       </c>
       <c r="I53" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="J53" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:22" ht="104.4" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B54" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="E54" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="F54" t="s">
         <v>38</v>
       </c>
       <c r="G54" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H54" t="s">
         <v>38</v>
@@ -4985,284 +5009,284 @@
         <v>17</v>
       </c>
       <c r="J54" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="K54" t="s">
         <v>44</v>
       </c>
       <c r="L54" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="55" spans="1:22" ht="104.4" x14ac:dyDescent="0.4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B55" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="E55" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F55" t="s">
         <v>15</v>
       </c>
       <c r="G55" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="H55" t="s">
         <v>38</v>
       </c>
       <c r="I55" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="J55" t="s">
         <v>38</v>
       </c>
       <c r="K55" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="L55" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="56" spans="1:22" ht="121.8" x14ac:dyDescent="0.4">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B56" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="E56" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F56" t="s">
         <v>8</v>
       </c>
       <c r="G56" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="H56" t="s">
         <v>8</v>
       </c>
       <c r="I56" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="J56" t="s">
         <v>8</v>
       </c>
       <c r="K56" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="L56" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:22" ht="295.8" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B57" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="E57" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F57" t="s">
         <v>38</v>
       </c>
       <c r="G57" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="H57" t="s">
         <v>38</v>
       </c>
       <c r="I57" t="s">
+        <v>308</v>
+      </c>
+      <c r="J57" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B58" t="s">
+        <v>311</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="E58" t="s">
+        <v>314</v>
+      </c>
+      <c r="F58" t="s">
+        <v>190</v>
+      </c>
+      <c r="G58" t="s">
+        <v>57</v>
+      </c>
+      <c r="H58" t="s">
+        <v>190</v>
+      </c>
+      <c r="I58" t="s">
         <v>315</v>
       </c>
-      <c r="J57" t="s">
+      <c r="J58" t="s">
+        <v>190</v>
+      </c>
+      <c r="K58" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="58" spans="1:22" ht="104.4" x14ac:dyDescent="0.4">
-      <c r="B58" t="s">
+      <c r="L58" t="s">
+        <v>190</v>
+      </c>
+      <c r="M58" t="s">
+        <v>317</v>
+      </c>
+      <c r="N58" t="s">
         <v>318</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="O58" t="s">
         <v>319</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="P58" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
         <v>320</v>
       </c>
-      <c r="E58" t="s">
+      <c r="B59" t="s">
+        <v>322</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="F58" t="s">
-        <v>197</v>
-      </c>
-      <c r="G58" t="s">
-        <v>59</v>
-      </c>
-      <c r="H58" t="s">
-        <v>197</v>
-      </c>
-      <c r="I58" t="s">
-        <v>322</v>
-      </c>
-      <c r="J58" t="s">
-        <v>197</v>
-      </c>
-      <c r="K58" t="s">
+      <c r="D59" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="L58" t="s">
-        <v>197</v>
-      </c>
-      <c r="M58" t="s">
+      <c r="E59" t="s">
+        <v>316</v>
+      </c>
+      <c r="F59" t="s">
         <v>324</v>
       </c>
-      <c r="N58" t="s">
-        <v>325</v>
-      </c>
-      <c r="O58" t="s">
-        <v>326</v>
-      </c>
-      <c r="P58" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="59" spans="1:22" ht="69.599999999999994" x14ac:dyDescent="0.4">
-      <c r="A59" t="s">
-        <v>327</v>
-      </c>
-      <c r="B59" t="s">
-        <v>329</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="E59" t="s">
-        <v>323</v>
-      </c>
-      <c r="F59" t="s">
-        <v>331</v>
-      </c>
       <c r="G59" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="H59" t="s">
         <v>8</v>
       </c>
       <c r="I59" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="J59" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:22" ht="409.6" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="E60" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F60" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="G60" t="s">
         <v>23</v>
       </c>
       <c r="H60" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="I60" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="J60" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="61" spans="1:22" ht="87" x14ac:dyDescent="0.4">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="E61" t="s">
         <v>23</v>
       </c>
       <c r="F61" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="G61" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H61" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="I61" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="J61" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="K61" s="3" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="L61" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="62" spans="1:22" ht="69.599999999999994" x14ac:dyDescent="0.4">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="E62" t="s">
         <v>37</v>
       </c>
       <c r="F62" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="H62" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I62" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J62" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="K62" t="s">
         <v>25</v>
@@ -5271,15 +5295,15 @@
         <v>18</v>
       </c>
       <c r="M62" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="63" spans="1:22" ht="52.2" x14ac:dyDescent="0.4">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="E63" t="s">
         <v>37</v>
@@ -5288,74 +5312,74 @@
         <v>38</v>
       </c>
       <c r="G63" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="H63" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I63" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="J63" t="s">
         <v>38</v>
       </c>
       <c r="K63" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="L63" t="s">
         <v>38</v>
       </c>
       <c r="M63" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B64" t="s">
+        <v>349</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E64" t="s">
+        <v>316</v>
+      </c>
+      <c r="F64" t="s">
+        <v>191</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="H64" t="s">
+        <v>191</v>
+      </c>
+      <c r="I64" t="s">
+        <v>343</v>
+      </c>
+      <c r="J64" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B65" t="s">
+        <v>353</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="64" spans="1:22" ht="208.8" x14ac:dyDescent="0.4">
-      <c r="B64" t="s">
-        <v>356</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="E64" t="s">
-        <v>323</v>
-      </c>
-      <c r="F64" t="s">
-        <v>198</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="H64" t="s">
-        <v>198</v>
-      </c>
-      <c r="I64" t="s">
-        <v>350</v>
-      </c>
-      <c r="J64" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" ht="139.19999999999999" x14ac:dyDescent="0.4">
-      <c r="B65" t="s">
-        <v>360</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>361</v>
-      </c>
       <c r="D65" s="3" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="E65" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="F65" t="s">
         <v>8</v>
       </c>
       <c r="G65" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H65" t="s">
         <v>8</v>
@@ -5373,190 +5397,190 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="156.6" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="E66" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="F66" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G66" t="s">
         <v>37</v>
       </c>
       <c r="H66" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="I66" t="s">
         <v>16</v>
       </c>
       <c r="J66" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" ht="52.2" x14ac:dyDescent="0.4">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B67" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="E67" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="F67" t="s">
         <v>22</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="H67" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" ht="121.8" x14ac:dyDescent="0.4">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B68" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="E68" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="F68" t="s">
         <v>8</v>
       </c>
       <c r="G68" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H68" t="s">
         <v>8</v>
       </c>
       <c r="I68" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="J68" t="s">
         <v>8</v>
       </c>
       <c r="K68" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="L68" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="174" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B69" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="E69" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="F69" t="s">
         <v>29</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="H69" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="I69" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="J69" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" ht="156.6" x14ac:dyDescent="0.4">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B70" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="E70" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="F70" t="s">
         <v>38</v>
       </c>
       <c r="G70" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="H70" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="I70" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="J70" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="K70" t="s">
         <v>16</v>
       </c>
       <c r="L70" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="M70" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="N70" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="139.19999999999999" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="E71" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="F71" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G71" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="H71" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="I71" t="s">
         <v>37</v>
       </c>
       <c r="J71" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="K71" t="s">
         <v>16</v>
@@ -5565,53 +5589,53 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="104.4" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B72" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="E72" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="F72" t="s">
         <v>22</v>
       </c>
       <c r="G72" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="H72" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" ht="191.4" x14ac:dyDescent="0.4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="B73" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="E73" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="F73" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="G73" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="H73" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="I73" t="s">
         <v>25</v>
@@ -5620,21 +5644,21 @@
         <v>8</v>
       </c>
       <c r="K73" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="L73" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="87" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B74" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="E74" t="s">
         <v>25</v>
@@ -5643,103 +5667,103 @@
         <v>8</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="H74" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" ht="382.8" x14ac:dyDescent="0.4">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B75" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="E75" t="s">
         <v>16</v>
       </c>
       <c r="F75" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="G75" t="s">
         <v>23</v>
       </c>
       <c r="H75" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="I75" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="J75" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" ht="226.2" x14ac:dyDescent="0.4">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B76" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="E76" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="F76" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="G76" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="H76" t="s">
         <v>18</v>
       </c>
       <c r="I76" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="J76" t="s">
         <v>18</v>
       </c>
       <c r="K76" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="L76" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="M76" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="N76" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="139.19999999999999" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B77" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="E77" t="s">
         <v>23</v>
       </c>
       <c r="F77" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G77" t="s">
         <v>16</v>
       </c>
       <c r="H77" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="I77" t="s">
         <v>17</v>
@@ -5748,10 +5772,10 @@
         <v>18</v>
       </c>
       <c r="K77" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="L77" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>